<commit_message>
part2 output format fix
</commit_message>
<xml_diff>
--- a/data/part2/PM10_п.xlsx
+++ b/data/part2/PM10_п.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Станция</t>
   </si>
@@ -32,40 +32,10 @@
     <t>Период превышения &amp;quot;ПО&amp;quot;</t>
   </si>
   <si>
-    <t>Зеленоград 16</t>
+    <t>Технополис</t>
   </si>
   <si>
-    <t>18/09/2024 08:20</t>
-  </si>
-  <si>
-    <t>18/09/2024 08:40</t>
-  </si>
-  <si>
-    <t>Долгопрудная</t>
-  </si>
-  <si>
-    <t>18/09/2024 19:20</t>
-  </si>
-  <si>
-    <t>18/09/2024 20:00</t>
-  </si>
-  <si>
-    <t>19/09/2024 02:00</t>
-  </si>
-  <si>
-    <t>Черемушки</t>
-  </si>
-  <si>
-    <t>18/09/2024 22:00</t>
-  </si>
-  <si>
-    <t>М1 (Очаковское)</t>
-  </si>
-  <si>
-    <t>19/09/2024 07:00</t>
-  </si>
-  <si>
-    <t>19/09/2024 07:20</t>
+    <t>21/10/2024 19:20</t>
   </si>
 </sst>
 </file>
@@ -208,81 +178,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="n">
         <v>6</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>